<commit_message>
Validated survey case study; changes through 9/26 11:55
</commit_message>
<xml_diff>
--- a/tests/test_data/tbl1_survey.xlsx
+++ b/tests/test_data/tbl1_survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Box Sync\Projects\Python_ProjTables\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A755F3B-C863-4A5E-9907-B85E2F1A18AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31A14C2-719D-464E-8549-5DAD790907AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="1785" windowWidth="35243" windowHeight="14265" xr2:uid="{0EE3CDFA-1153-4088-A8D0-88624F64512D}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="11332" xr2:uid="{0EE3CDFA-1153-4088-A8D0-88624F64512D}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_table" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Answer Choices</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>Habit Survey (Survey Monkey Question format)</t>
+  </si>
+  <si>
+    <t>Lower price point</t>
+  </si>
+  <si>
+    <t>Q3. How would you improve your current product (Rank 1 to 3)</t>
+  </si>
+  <si>
+    <t>Better package</t>
+  </si>
+  <si>
+    <t>Improved cleaning</t>
   </si>
 </sst>
 </file>
@@ -480,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3523742-792E-40AB-A946-ADD54C769B65}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -612,7 +624,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -623,7 +635,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -634,7 +646,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>13</v>
       </c>
@@ -642,12 +654,73 @@
         <v>538</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>14</v>
       </c>
       <c r="C20">
         <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>91</v>
+      </c>
+      <c r="C26">
+        <v>33</v>
+      </c>
+      <c r="D26">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <v>37</v>
+      </c>
+      <c r="D27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>18</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>